<commit_message>
[*]新增NOTE欄位合併儲存格 [*]修正Order Number髒資料 [*]把系統產出的報表appen到廠商提供excel的分頁後面 [+]sweet alert [+]upload info display [*]s18 OrderNo用Regex.Replace去特殊字元 [*]大18 excel檢核是否為空白列 [+]增加ExceptionFilterAttribute，捕捉api回傳型別不是Result的api(ex: excel export) [*]maxAllowedContentLength上限修改為100MB，並增加上傳前檢核 [+]新增vt01. vt02. prd設定檔 [*]修改上傳路徑，避免實體路徑全部顯示 [+]add ELMAHCore
</commit_message>
<xml_diff>
--- a/LCM.Website/Content/PK_Report_Template.xlsx
+++ b/LCM.Website/Content/PK_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38508" yWindow="-15216" windowWidth="38616" windowHeight="21096"/>
+    <workbookView xWindow="-38508" yWindow="-15216" windowWidth="38616" windowHeight="21096" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Closed" sheetId="6" r:id="rId1"/>
@@ -269,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,12 +279,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,7 +392,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,34 +402,28 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
@@ -444,23 +432,17 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -751,44 +733,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="14" style="14" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.77734375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" style="14" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" style="14" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" style="14" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" style="14" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="20" customWidth="1"/>
-    <col min="15" max="15" width="19.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" style="14" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" style="14" customWidth="1"/>
-    <col min="19" max="19" width="8.77734375" style="14"/>
-    <col min="20" max="20" width="9.88671875" style="14" customWidth="1"/>
-    <col min="21" max="21" width="24" style="14" customWidth="1"/>
-    <col min="22" max="22" width="12" style="14" customWidth="1"/>
-    <col min="23" max="23" width="16.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="12" style="14" customWidth="1"/>
-    <col min="27" max="27" width="15.44140625" style="14" customWidth="1"/>
-    <col min="28" max="35" width="0" style="14" hidden="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.77734375" style="14"/>
+    <col min="1" max="1" width="14" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.77734375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="14" customWidth="1"/>
+    <col min="15" max="15" width="19.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" style="12" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" style="12" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" style="12"/>
+    <col min="20" max="20" width="9.88671875" style="12" customWidth="1"/>
+    <col min="21" max="21" width="24" style="12" customWidth="1"/>
+    <col min="22" max="22" width="12" style="12" customWidth="1"/>
+    <col min="23" max="23" width="16.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="12" style="12" customWidth="1"/>
+    <col min="27" max="27" width="15.44140625" style="12" customWidth="1"/>
+    <col min="28" max="35" width="0" style="12" hidden="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.77734375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="26.4" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,10 +810,10 @@
       <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -871,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="4" customFormat="1">
+    <row r="2" spans="1:27" s="3" customFormat="1" ht="26.4" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
@@ -887,7 +869,7 @@
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="16"/>
@@ -904,90 +886,94 @@
       <c r="Z2" s="16"/>
       <c r="AA2" s="16"/>
     </row>
-    <row r="3" spans="1:27" s="13" customFormat="1" ht="41.4">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:27" s="11" customFormat="1" ht="26.4" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="V3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="X3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Z3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="10" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="N2:AA2"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -998,44 +984,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="14" style="14" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.77734375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" style="14" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" style="14" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" style="14" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" style="14" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="20" customWidth="1"/>
-    <col min="15" max="15" width="19.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" style="14" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" style="14" customWidth="1"/>
-    <col min="19" max="19" width="8.77734375" style="14"/>
-    <col min="20" max="20" width="9.88671875" style="14" customWidth="1"/>
-    <col min="21" max="21" width="24" style="14" customWidth="1"/>
-    <col min="22" max="22" width="12" style="14" customWidth="1"/>
-    <col min="23" max="23" width="16.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="12" style="14" customWidth="1"/>
-    <col min="27" max="27" width="15.33203125" style="14" customWidth="1"/>
-    <col min="28" max="32" width="0" style="14" hidden="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.77734375" style="14"/>
+    <col min="1" max="1" width="14" style="12" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.77734375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="14" customWidth="1"/>
+    <col min="15" max="15" width="19.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" style="12" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" style="12" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" style="12"/>
+    <col min="20" max="20" width="9.88671875" style="12" customWidth="1"/>
+    <col min="21" max="21" width="24" style="12" customWidth="1"/>
+    <col min="22" max="22" width="12" style="12" customWidth="1"/>
+    <col min="23" max="23" width="16.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="12" style="12" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" style="12" customWidth="1"/>
+    <col min="28" max="32" width="0" style="12" hidden="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.77734375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="21" customHeight="1">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="26.4" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1075,10 +1061,10 @@
       <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1118,7 +1104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="4" customFormat="1">
+    <row r="2" spans="1:27" s="3" customFormat="1" ht="26.4" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
@@ -1134,7 +1120,7 @@
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="16"/>
@@ -1151,90 +1137,94 @@
       <c r="Z2" s="16"/>
       <c r="AA2" s="16"/>
     </row>
-    <row r="3" spans="1:27" s="13" customFormat="1" ht="41.4">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:27" s="11" customFormat="1" ht="26.4" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="V3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="X3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Y3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="Z3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="10" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="N2:AA2"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1242,6 +1232,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c985b55e-824b-4be8-ac02-9996eda26dda" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7630c48-9f04-4150-8691-5031263a0d91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006110D2F5B2E5214A9B9E7F50C40DB167" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eca471b134068a5643084444d07f0b9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e7630c48-9f04-4150-8691-5031263a0d91" xmlns:ns3="c985b55e-824b-4be8-ac02-9996eda26dda" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9c6ad9ada77510d01125813ba3a74df5" ns2:_="" ns3:_="">
     <xsd:import namespace="e7630c48-9f04-4150-8691-5031263a0d91"/>
@@ -1418,27 +1428,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8A4FAB0-596D-491A-BC20-AFAB8ACF69FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c985b55e-824b-4be8-ac02-9996eda26dda" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7630c48-9f04-4150-8691-5031263a0d91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99B46D63-1B93-4301-A254-6276C2180BE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c985b55e-824b-4be8-ac02-9996eda26dda"/>
+    <ds:schemaRef ds:uri="e7630c48-9f04-4150-8691-5031263a0d91"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{386AB303-938F-47B0-ABDA-A224B7D42171}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1455,23 +1464,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8A4FAB0-596D-491A-BC20-AFAB8ACF69FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99B46D63-1B93-4301-A254-6276C2180BE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c985b55e-824b-4be8-ac02-9996eda26dda"/>
-    <ds:schemaRef ds:uri="e7630c48-9f04-4150-8691-5031263a0d91"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>